<commit_message>
Fixed popup menu style
</commit_message>
<xml_diff>
--- a/localizations.xlsx
+++ b/localizations.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Grade.ly\Grade.ly - Flutter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A9A650-73EB-4852-A0A2-BAA8695598BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{416BD51D-261A-4BC8-BC38-306D87CA65B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="string" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0">string!$A$1:$B$95</definedName>
+    <definedName name="ExternalData_1" localSheetId="0">string!$A$1:$B$96</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="396">
   <si>
     <t>keys</t>
   </si>
@@ -1196,6 +1196,21 @@
   </si>
   <si>
     <t>Maximum</t>
+  </si>
+  <si>
+    <t>more_options</t>
+  </si>
+  <si>
+    <t>More options</t>
+  </si>
+  <si>
+    <t>Plus d'options</t>
+  </si>
+  <si>
+    <t>Mehr Optionen</t>
+  </si>
+  <si>
+    <t>Méi Optiounen</t>
   </si>
 </sst>
 </file>
@@ -1253,8 +1268,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="string" displayName="string" ref="A1:E95" totalsRowShown="0">
-  <autoFilter ref="A1:E95" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="string" displayName="string" ref="A1:E96" totalsRowShown="0">
+  <autoFilter ref="A1:E96" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="keys"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="en"/>
@@ -1554,10 +1569,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E95"/>
+  <dimension ref="A1:E96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="A95" sqref="A95:XFD95"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="E96" sqref="E96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1566,7 +1581,7 @@
     <col min="2" max="2" width="29.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="52.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3182,6 +3197,23 @@
       </c>
       <c r="E95" s="2" t="s">
         <v>390</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>395</v>
       </c>
     </row>
   </sheetData>

</xml_diff>